<commit_message>
ordenar tabs en reporte
</commit_message>
<xml_diff>
--- a/public_html/admin/reportesgenerados/Memberships-87.xlsx
+++ b/public_html/admin/reportesgenerados/Memberships-87.xlsx
@@ -32,7 +32,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Corina Segundo,  Jorge Fernández,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf</t>
+          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Corina Segundo,  Jorge Fernández,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic</t>
         </r>
       </text>
     </comment>
@@ -80,7 +80,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  Tomás Vega,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf</t>
+          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  Tomás Vega,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco</t>
         </r>
       </text>
     </comment>
@@ -128,7 +128,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  Tomás Vega,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Santiago Reyna,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Eduardo Arnillas,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf</t>
+          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  Tomás Vega,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Santiago Reyna,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Eduardo Arnillas,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco</t>
         </r>
       </text>
     </comment>
@@ -176,7 +176,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  Tomás Vega,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Santiago Reyna,  Luis Rivera,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Eduardo Arnillas,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Olazhir Ledezma,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  David Testing 1,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf</t>
+          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  David Testing 1,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  Tomás Vega,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Santiago Reyna,  Luis Rivera,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Eduardo Arnillas,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Olazhir Ledezma,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco</t>
         </r>
       </text>
     </comment>
@@ -224,7 +224,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Santiago Reyna,  Luis Rivera,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Eduardo Arnillas,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Olazhir Ledezma,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  David Testing 1,  Jose del Rio,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf</t>
+          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  David Testing 1,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Santiago Reyna,  Luis Rivera,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Eduardo Arnillas,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Olazhir Ledezma,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  Jose del Rio</t>
         </r>
       </text>
     </comment>
@@ -272,7 +272,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Juan Alberto Forsyth,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Juan Antonio Rozas,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Santiago Reyna,  Luis Rivera,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Eduardo Arnillas,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Olazhir Ledezma,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  David Testing 1,  Jose del Rio,  apli4 apli4,  apli7 apli7,  Juan Alberto Forsyth,  Juan Alberto Forsyth,  Jorge Luis Feliú,  pru3 pru3,  apli6 apli6,  aplicante12 aplicante12,  apli3 apli3,  aplicantepru aplicantepru,  asdfasdf asdfasdfasdf</t>
+          <t xml:space="preserve"> Juan Alberto Forsyth,  Juan Alberto Forsyth,  Juan Alberto Forsyth,  Jorge Luis Feliú,  Jorge Luis Feliú,  Eduardo Wichtel,  Michel Michell,  Jorge Ramos,  Humberto Chávez,  Rolando Giha,  David Testing 1,  aplicantepru aplicantepru,  aplicante12 aplicante12,  apli3 apli3,  apli4 apli4,  apli6 apli6,  apli7 apli7,  pru3 pru3,  asdfasdf asdfasdfasdf,  Edgardo Vargas,  Rafael Treistman,  Guy Fort,  Juan Gabriel Reyes,  Jaime Yoshiyama,  Alberto Pinto,  José Borda,  Luis Vargas,  Ricardo Arce,  José Ackerman,  Mario Campodónico,  Manuel Gallofré,  Félix Antelo,  Carlos Mujica,  Michel Steiert,  Marco Peschiera,  Reynaldo Llosa,  Alfonzo Vásquez,  Diego Rey,  Jeanine Mellet,  Eduardo Carriquiery,  Juan Antonio Rozas,  Gonzalo Van Oordt,  Willard Manrique,  Javier Zegarra,  Bruno Novella,  Carlos Caro,  Luis Antonio Aspillaga,  Ricardo Maldonado,  Maritza Reátegui,  Carl Rooth,  Roberto Taboada,  Alejandro Ormeño,  Carlos Morante,  Alejandro Amaya,  Piero Bengoa,  Percy Ortiz,  Jaime Atun,  Santiago Reyna,  Luis Rivera,  Raúl Espinoza,  Christian Neuhaus,  Javier Delgado,  Diego Aguirre,  Alfonso Panizo,  Daniel Linares,  Igor Salazar,  Mirella Velásquez,  Alvaro Merino Reyna,  Miryam Mesía,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Enrique Garland,  Fernando Herrera,  Guillermo Winter,  José Orrego,  Katherina Exebio,  Giovanni Klein,  Mónica Eyzaguirre,  Javier Draxl,  Percy Castle,  Ralph Guerra,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Corina Segundo,  Jorge Fernández,  Eduardo Arnillas,  Raúl Barrios,  Pedro Gomes,  Alfonso de la Piedra,  Olazhir Ledezma,  Marie Rosso,  Madeleine Osterling,  Verónica Arbulú,  Anita Belaúnde,  Frida Delgado,  Ursula Mercado,  Ana María Campos,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  Jose del Rio</t>
         </r>
       </text>
     </comment>
@@ -528,7 +528,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Michel Michell,  Tomás Vega,  Carlos Caro,  Santiago Reyna,  Luis Rivera,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Jorge Fernández,  Eduardo Arnillas,  Alfonso de la Piedra,  Olazhir Ledezma,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  David Testing 1</t>
+          <t xml:space="preserve"> Michel Michell,  David Testing 1,  Tomás Vega,  Carlos Caro,  Santiago Reyna,  Luis Rivera,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Jorge Fernández,  Eduardo Arnillas,  Alfonso de la Piedra,  Olazhir Ledezma,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco</t>
         </r>
       </text>
     </comment>
@@ -560,7 +560,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Michel Michell,  Tomás Vega,  Carlos Caro,  Santiago Reyna,  Luis Rivera,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Jorge Fernández,  Eduardo Arnillas,  Alfonso de la Piedra,  Olazhir Ledezma,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  David Testing 1,  Jose del Rio</t>
+          <t xml:space="preserve"> Michel Michell,  David Testing 1,  Tomás Vega,  Carlos Caro,  Santiago Reyna,  Luis Rivera,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Jorge Fernández,  Eduardo Arnillas,  Alfonso de la Piedra,  Olazhir Ledezma,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  Jose del Rio</t>
         </r>
       </text>
     </comment>
@@ -592,7 +592,7 @@
             <sz val="11"/>
             <u val="none"/>
           </rPr>
-          <t xml:space="preserve"> Michel Michell,  Tomás Vega,  Juan Antonio Rozas,  Carlos Caro,  Santiago Reyna,  Luis Rivera,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Jorge Fernández,  Eduardo Arnillas,  Alfonso de la Piedra,  Olazhir Ledezma,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  David Testing 1,  Jose del Rio,  apli4 apli4,  apli7 apli7,  Juan Alberto Forsyth,  Juan Alberto Forsyth,  Jorge Luis Feliú,  pru3 pru3,  apli6 apli6,  aplicante12 aplicante12,  apli3 apli3</t>
+          <t xml:space="preserve"> Juan Alberto Forsyth,  Juan Alberto Forsyth,  Jorge Luis Feliú,  Michel Michell,  David Testing 1,  aplicante12 aplicante12,  apli3 apli3,  apli4 apli4,  apli6 apli6,  apli7 apli7,  pru3 pru3,  Tomás Vega,  Juan Antonio Rozas,  Carlos Caro,  Santiago Reyna,  Luis Rivera,  Daniel Vaillant,  José Luis Hidalgo,  Jorge Carbajal,  Luis Miguel Peña,  Claudia Medina,  Edgardo Malpartida,  Guillermo León Velarde,  Rohit Rao,  Victor Vignale,  Jorge Fernández,  Eduardo Arnillas,  Alfonso de la Piedra,  Olazhir Ledezma,  Julia Sobrevilla,  Alberto Morillo,  Craig Smith,  Fernando Farah,  José Antonio Roca,  Franjo Kurtovic,  Simón Fishman,  José Cuenco,  Jose del Rio</t>
         </r>
       </text>
     </comment>
@@ -606,7 +606,7 @@
     <t>RODOLFO BAQUERIZO</t>
   </si>
   <si>
-    <t>2017 - 04/10/2017</t>
+    <t>2017 - 17/10/2017</t>
   </si>
   <si>
     <t>Top Executive</t>

</xml_diff>